<commit_message>
Focntion de login implémentée et MCD établi
</commit_message>
<xml_diff>
--- a/Doc/Journal de Travail.xlsx
+++ b/Doc/Journal de Travail.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC Nolan\OneDrive - CPNV\1ere Année\CFC\ICT-431\Bataille Navale\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Apprentissage\1re annee\2e Trimestre\MA-20\Bataille_Navale\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EBF9BC4-4198-4E7A-A292-ECF837BFF6A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA40DDAB-8F5F-4C8B-AE59-0A63623EB474}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="113">
   <si>
     <t>Date</t>
   </si>
@@ -329,6 +329,36 @@
   </si>
   <si>
     <t>Ecriture du README et finalisation de la documentation</t>
+  </si>
+  <si>
+    <t>Résolution d'un bug d'affichage de map</t>
+  </si>
+  <si>
+    <t>23.03.2020</t>
+  </si>
+  <si>
+    <t>Réajustement des dimensions de la map</t>
+  </si>
+  <si>
+    <t>25.03.2020</t>
+  </si>
+  <si>
+    <t>12h00</t>
+  </si>
+  <si>
+    <t>Correction sprint 4 et création du sprint 5</t>
+  </si>
+  <si>
+    <t>26.03.2020</t>
+  </si>
+  <si>
+    <t>9h15</t>
+  </si>
+  <si>
+    <t>75 min</t>
+  </si>
+  <si>
+    <t>Implémentation fonction de login</t>
   </si>
 </sst>
 </file>
@@ -662,7 +692,7 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1602,46 +1632,102 @@
       <c r="I37" s="5"/>
     </row>
     <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="3"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="9"/>
+      <c r="A38" s="3">
+        <v>43909</v>
+      </c>
+      <c r="B38" s="7">
+        <v>4</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>103</v>
+      </c>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
     </row>
     <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="3"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="9"/>
+      <c r="A39" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B39" s="4">
+        <v>5</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>105</v>
+      </c>
       <c r="H39" s="5"/>
       <c r="I39" s="6"/>
     </row>
     <row r="40" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="3"/>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="9"/>
+      <c r="A40" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B40" s="7">
+        <v>5</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>108</v>
+      </c>
       <c r="H40" s="5"/>
       <c r="I40" s="6"/>
     </row>
     <row r="41" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A41" s="3"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="9"/>
+      <c r="A41" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B41" s="7">
+        <v>5</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>112</v>
+      </c>
       <c r="H41" s="5"/>
       <c r="I41" s="6"/>
     </row>

</xml_diff>

<commit_message>
système de logs et bibliothèques de plans de jeu implémentés
</commit_message>
<xml_diff>
--- a/Doc/Journal de Travail.xlsx
+++ b/Doc/Journal de Travail.xlsx
@@ -8,19 +8,29 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Apprentissage\1re annee\2e Trimestre\MA-20\Bataille_Navale\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA40DDAB-8F5F-4C8B-AE59-0A63623EB474}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F5CC359-783A-4A9B-BE3D-CC64915EDE7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="119">
   <si>
     <t>Date</t>
   </si>
@@ -360,6 +370,24 @@
   <si>
     <t>Implémentation fonction de login</t>
   </si>
+  <si>
+    <t>17h00</t>
+  </si>
+  <si>
+    <t>Ecriture des trois premiers plans de jeu</t>
+  </si>
+  <si>
+    <t>01.04.2020</t>
+  </si>
+  <si>
+    <t>10h15</t>
+  </si>
+  <si>
+    <t>Implémentation du système de logs</t>
+  </si>
+  <si>
+    <t>Etablissement du sprint 6</t>
+  </si>
 </sst>
 </file>
 
@@ -691,8 +719,8 @@
   </sheetPr>
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G44" sqref="G44"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1732,35 +1760,77 @@
       <c r="I41" s="6"/>
     </row>
     <row r="42" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A42" s="3"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="9"/>
+      <c r="A42" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B42" s="7">
+        <v>5</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>114</v>
+      </c>
       <c r="H42" s="5"/>
       <c r="I42" s="6"/>
     </row>
     <row r="43" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="3"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="9"/>
+      <c r="A43" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B43" s="4">
+        <v>6</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>117</v>
+      </c>
       <c r="H43" s="5"/>
       <c r="I43" s="6"/>
     </row>
     <row r="44" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A44" s="3"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="9"/>
+      <c r="A44" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B44" s="7">
+        <v>6</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G44" s="9" t="s">
+        <v>118</v>
+      </c>
       <c r="H44" s="5"/>
       <c r="I44" s="6"/>
     </row>

</xml_diff>